<commit_message>
Readme extra tekst toegevoegd ter uitleg clean report. Fix voor streepjes die ? worden. Open EAD gefixt. KWStoExcel: urogen en vasc toegevoegd Cases.xlsx opgekuist en format.
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mixer\home50\cvmarc2\uzlsystem\Bureaublad\Autohotkey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mixer\home50\cvmarc2\uzlsystem\Bureaublad\Autohotkey\GIT\KWS-helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943260DF-C69A-4F0D-B668-B5952840517F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4957EFF4-13D7-41E9-94A9-61D400C9DAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="840" windowWidth="21600" windowHeight="11385" xr2:uid="{652A8BE9-BAFF-4435-BEB8-08795CEB1C68}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{652A8BE9-BAFF-4435-BEB8-08795CEB1C68}"/>
   </bookViews>
   <sheets>
     <sheet name="DB" sheetId="1" r:id="rId1"/>
-    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DB!$A$1:$H$7</definedName>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>EAD</t>
   </si>
@@ -53,9 +52,6 @@
     <t>Opmerking</t>
   </si>
   <si>
-    <t>Op te volgen?</t>
-  </si>
-  <si>
     <t>Onderzoek</t>
   </si>
   <si>
@@ -65,58 +61,10 @@
     <t>Diagn Vr.</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Beeld van subconjunctivale prolaps bij hypertrofie van het orbitale vet. Geringe propotose beiderzijds en aanwezigheid van atrofische externe oogspieren. Beeld kan passen in het kader van hypercortisolisme (exogeen/endogeen), doorgemaakt thyroidorbitopathie of in het kader van obesitas.</t>
-  </si>
-  <si>
-    <t>Tips voor postop:</t>
-  </si>
-  <si>
-    <t>SWI is ook vrij T1 gewogen: methemoglobine zal dus wit zijn</t>
-  </si>
-  <si>
-    <t>Ook: een intraparenchym hematoom zal op SWI op bepaalde tijdstippen enkel perifeer suscebil vertonen --&gt; dus centraal kan nog hyper door methem</t>
-  </si>
-  <si>
-    <t>Collateral index:</t>
-  </si>
-  <si>
-    <t>alles ONDER 0,5 is "goed"</t>
-  </si>
-  <si>
-    <t>Xu di</t>
-  </si>
-  <si>
-    <t>Flair signaal sinys transversus: Ofwel trombose gehad, ofwel hypoplastisch --&gt; eerder hypoplastisch op CT</t>
-  </si>
-  <si>
-    <t>Doordat de flow wat anders gaat, met wat granulationes -&gt; Flair artefacten</t>
-  </si>
-  <si>
-    <t>Intraventr mening</t>
-  </si>
-  <si>
-    <t>Reden: oudere leeftijd tupisch plaats intraventr occ hoorn, of op oudere leeftijd infratentorieel ook meer</t>
-  </si>
-  <si>
-    <t>Ook calcificaties classic</t>
-  </si>
-  <si>
-    <t>ITT papilloom: ook Ca maar typisch bloemkool aflijning ( niet zo mooi bolrond als mening)</t>
-  </si>
-  <si>
-    <t>Ook hyperdense focus</t>
-  </si>
-  <si>
-    <t>Omdat wat lineair is kan het nog een DVA zijn</t>
-  </si>
-  <si>
-    <t>of cavernoom</t>
-  </si>
-  <si>
     <t>Tag</t>
+  </si>
+  <si>
+    <t>Op te volgen tegen</t>
   </si>
 </sst>
 </file>
@@ -169,7 +117,7 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -181,6 +129,13 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -196,14 +151,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{427F353C-C718-4D12-B2F1-D89E5B344F81}" name="Tabel2" displayName="Tabel2" ref="A1:I1048576" totalsRowShown="0">
-  <autoFilter ref="A1:I1048576" xr:uid="{427F353C-C718-4D12-B2F1-D89E5B344F81}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{427F353C-C718-4D12-B2F1-D89E5B344F81}" name="Tabel2" displayName="Tabel2" ref="A1:I1048575" totalsRowShown="0">
+  <autoFilter ref="A1:I1048575" xr:uid="{427F353C-C718-4D12-B2F1-D89E5B344F81}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0B82E458-A291-448B-8C79-037B9132EE65}" name="EAD"/>
     <tableColumn id="2" xr3:uid="{A5A4BF5F-B579-477B-BCC0-A72A0295D4F8}" name="Datum"/>
     <tableColumn id="3" xr3:uid="{A3A1345F-65C8-4913-909F-FD367F2CA964}" name="Discipline"/>
     <tableColumn id="4" xr3:uid="{D84F3E4E-DAAB-4947-AF1C-5450B9D2062C}" name="Opmerking"/>
-    <tableColumn id="5" xr3:uid="{2F0E21B3-A0E5-4A12-963A-81E72AB2521D}" name="Op te volgen?"/>
+    <tableColumn id="5" xr3:uid="{2F0E21B3-A0E5-4A12-963A-81E72AB2521D}" name="Op te volgen tegen"/>
     <tableColumn id="6" xr3:uid="{1A0F6952-4420-42CF-A5C2-F9B14D4EA8CA}" name="Onderzoek" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{B7C4210C-6789-4C77-B791-332F3DAC138E}" name="Kl Inlichtingen" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{164A6E97-1458-4BEB-9AEF-9575EB889C0D}" name="Diagn Vr." dataDxfId="1"/>
@@ -510,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74AF834-2A9A-4884-8378-CCAB4D4261D2}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,10 +476,10 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="132.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="76" style="5" customWidth="1"/>
+    <col min="8" max="8" width="37.42578125" style="5" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="5"/>
   </cols>
   <sheetData>
@@ -542,19 +497,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -584,7 +539,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -656,182 +611,121 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="4"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="F28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
-      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="E41" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E40:E1048575 E2:E37">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>AND(E2&lt;TODAY(), E2 &gt; 41000)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4716D0EE-AC44-43C1-98D7-71B0BE4BE6FC}">
-  <dimension ref="A4:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="111" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>82808056</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>